<commit_message>
update spawning temp estimate approach
</commit_message>
<xml_diff>
--- a/data/lake-geneva/lake-geneva-spawning.xlsx
+++ b/data/lake-geneva/lake-geneva-spawning.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taylor/SynologyDrive/Cisco-Climate-Change/Coregonine-DegreeDay-Modeling/data/lake-geneva/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taylor/SynologyDrive/Cisco-Climate-Change/Coregonine-Embryo-Modeling/data/lake-geneva/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BF6A106-AFAB-5E4D-90D7-49C9C5E53DE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7CB10E6-DDBF-4D4F-939E-301CB46E3FA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="37440" yWindow="7720" windowWidth="27680" windowHeight="17100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>year</t>
   </si>
@@ -46,6 +46,12 @@
   </si>
   <si>
     <t>spawn.abundance</t>
+  </si>
+  <si>
+    <t>total.abundance</t>
+  </si>
+  <si>
+    <t>percent.abundance</t>
   </si>
 </sst>
 </file>
@@ -379,10 +385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D53"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -391,9 +397,11 @@
     <col min="2" max="2" width="8.5" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.83203125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -406,8 +414,14 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2016</v>
       </c>
@@ -420,8 +434,14 @@
       <c r="D2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2">
+        <v>57</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2016</v>
       </c>
@@ -434,8 +454,14 @@
       <c r="D3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3">
+        <v>57</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2016</v>
       </c>
@@ -448,8 +474,14 @@
       <c r="D4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4">
+        <v>57</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2016</v>
       </c>
@@ -462,8 +494,14 @@
       <c r="D5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5">
+        <v>57</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2016</v>
       </c>
@@ -476,8 +514,14 @@
       <c r="D6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6">
+        <v>57</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2016</v>
       </c>
@@ -490,8 +534,14 @@
       <c r="D7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7">
+        <v>57</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2016</v>
       </c>
@@ -504,8 +554,14 @@
       <c r="D8">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8">
+        <v>57</v>
+      </c>
+      <c r="F8" s="1">
+        <v>15.789473684210526</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2016</v>
       </c>
@@ -518,8 +574,14 @@
       <c r="D9">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9">
+        <v>57</v>
+      </c>
+      <c r="F9" s="1">
+        <v>17.543859649122805</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2016</v>
       </c>
@@ -532,8 +594,14 @@
       <c r="D10">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10">
+        <v>57</v>
+      </c>
+      <c r="F10" s="1">
+        <v>15.789473684210526</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2016</v>
       </c>
@@ -546,8 +614,14 @@
       <c r="D11">
         <v>14</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11">
+        <v>57</v>
+      </c>
+      <c r="F11" s="1">
+        <v>24.561403508771928</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2016</v>
       </c>
@@ -560,8 +634,14 @@
       <c r="D12">
         <v>13</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E12">
+        <v>57</v>
+      </c>
+      <c r="F12" s="1">
+        <v>22.807017543859647</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2016</v>
       </c>
@@ -574,8 +654,14 @@
       <c r="D13">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E13">
+        <v>57</v>
+      </c>
+      <c r="F13" s="1">
+        <v>3.5087719298245612</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2016</v>
       </c>
@@ -588,8 +674,14 @@
       <c r="D14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E14">
+        <v>57</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2016</v>
       </c>
@@ -602,8 +694,14 @@
       <c r="D15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E15">
+        <v>57</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2017</v>
       </c>
@@ -616,8 +714,14 @@
       <c r="D16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16">
+        <v>71</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2017</v>
       </c>
@@ -630,8 +734,14 @@
       <c r="D17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17">
+        <v>71</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1.4084507042253522</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2017</v>
       </c>
@@ -644,8 +754,14 @@
       <c r="D18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18">
+        <v>71</v>
+      </c>
+      <c r="F18" s="1">
+        <v>1.4084507042253522</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2017</v>
       </c>
@@ -658,8 +774,14 @@
       <c r="D19">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E19">
+        <v>71</v>
+      </c>
+      <c r="F19" s="1">
+        <v>7.042253521126761</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2017</v>
       </c>
@@ -672,8 +794,14 @@
       <c r="D20">
         <v>14</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E20">
+        <v>71</v>
+      </c>
+      <c r="F20" s="1">
+        <v>19.718309859154928</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2017</v>
       </c>
@@ -686,8 +814,14 @@
       <c r="D21">
         <v>16</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E21">
+        <v>71</v>
+      </c>
+      <c r="F21" s="1">
+        <v>22.535211267605636</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2017</v>
       </c>
@@ -700,8 +834,14 @@
       <c r="D22">
         <v>14</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E22">
+        <v>71</v>
+      </c>
+      <c r="F22" s="1">
+        <v>19.718309859154928</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2017</v>
       </c>
@@ -714,8 +854,14 @@
       <c r="D23">
         <v>8</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E23">
+        <v>71</v>
+      </c>
+      <c r="F23" s="1">
+        <v>11.267605633802818</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>2017</v>
       </c>
@@ -728,8 +874,14 @@
       <c r="D24">
         <v>3</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E24">
+        <v>71</v>
+      </c>
+      <c r="F24" s="1">
+        <v>4.225352112676056</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2017</v>
       </c>
@@ -742,8 +894,14 @@
       <c r="D25">
         <v>5</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E25">
+        <v>71</v>
+      </c>
+      <c r="F25" s="1">
+        <v>7.042253521126761</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2017</v>
       </c>
@@ -756,8 +914,14 @@
       <c r="D26">
         <v>2</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E26">
+        <v>71</v>
+      </c>
+      <c r="F26" s="1">
+        <v>2.8169014084507045</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2017</v>
       </c>
@@ -770,8 +934,14 @@
       <c r="D27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E27">
+        <v>71</v>
+      </c>
+      <c r="F27" s="1">
+        <v>1.4084507042253522</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>2017</v>
       </c>
@@ -784,8 +954,14 @@
       <c r="D28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E28">
+        <v>71</v>
+      </c>
+      <c r="F28" s="1">
+        <v>1.4084507042253522</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>2017</v>
       </c>
@@ -798,8 +974,14 @@
       <c r="D29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E29">
+        <v>71</v>
+      </c>
+      <c r="F29" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>2018</v>
       </c>
@@ -812,8 +994,14 @@
       <c r="D30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E30">
+        <v>23</v>
+      </c>
+      <c r="F30" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>2018</v>
       </c>
@@ -826,8 +1014,14 @@
       <c r="D31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E31">
+        <v>23</v>
+      </c>
+      <c r="F31" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>2018</v>
       </c>
@@ -840,8 +1034,14 @@
       <c r="D32">
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E32">
+        <v>23</v>
+      </c>
+      <c r="F32" s="1">
+        <v>8.695652173913043</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>2018</v>
       </c>
@@ -854,8 +1054,14 @@
       <c r="D33" s="6">
         <v>5</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E33">
+        <v>23</v>
+      </c>
+      <c r="F33" s="1">
+        <v>21.739130434782609</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>2018</v>
       </c>
@@ -868,8 +1074,14 @@
       <c r="D34" s="6">
         <v>5</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E34">
+        <v>23</v>
+      </c>
+      <c r="F34" s="1">
+        <v>21.739130434782609</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>2018</v>
       </c>
@@ -882,8 +1094,14 @@
       <c r="D35" s="6">
         <v>6</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E35">
+        <v>23</v>
+      </c>
+      <c r="F35" s="1">
+        <v>26.086956521739129</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>2018</v>
       </c>
@@ -894,8 +1112,14 @@
       <c r="D36" s="6">
         <v>3</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E36">
+        <v>23</v>
+      </c>
+      <c r="F36" s="1">
+        <v>13.043478260869565</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>2018</v>
       </c>
@@ -906,8 +1130,14 @@
       <c r="D37" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E37">
+        <v>23</v>
+      </c>
+      <c r="F37" s="1">
+        <v>8.695652173913043</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>2018</v>
       </c>
@@ -920,8 +1150,14 @@
       <c r="D38" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E38">
+        <v>23</v>
+      </c>
+      <c r="F38" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>2018</v>
       </c>
@@ -934,8 +1170,14 @@
       <c r="D39" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E39">
+        <v>23</v>
+      </c>
+      <c r="F39" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>2018</v>
       </c>
@@ -948,8 +1190,14 @@
       <c r="D40" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E40">
+        <v>23</v>
+      </c>
+      <c r="F40" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>2018</v>
       </c>
@@ -962,8 +1210,14 @@
       <c r="D41" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E41">
+        <v>23</v>
+      </c>
+      <c r="F41" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>2018</v>
       </c>
@@ -976,8 +1230,14 @@
       <c r="D42" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E42">
+        <v>23</v>
+      </c>
+      <c r="F42" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>2018</v>
       </c>
@@ -990,8 +1250,14 @@
       <c r="D43" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E43">
+        <v>23</v>
+      </c>
+      <c r="F43" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>2019</v>
       </c>
@@ -1004,8 +1270,14 @@
       <c r="D44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E44">
+        <v>26</v>
+      </c>
+      <c r="F44" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>2019</v>
       </c>
@@ -1018,8 +1290,14 @@
       <c r="D45">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E45">
+        <v>26</v>
+      </c>
+      <c r="F45" s="1">
+        <v>3.8461538461538463</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>2019</v>
       </c>
@@ -1032,8 +1310,14 @@
       <c r="D46">
         <v>4</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E46">
+        <v>26</v>
+      </c>
+      <c r="F46" s="1">
+        <v>15.384615384615385</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>2019</v>
       </c>
@@ -1046,8 +1330,14 @@
       <c r="D47" s="6">
         <v>8</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E47">
+        <v>26</v>
+      </c>
+      <c r="F47" s="1">
+        <v>30.76923076923077</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>2019</v>
       </c>
@@ -1060,8 +1350,14 @@
       <c r="D48" s="6">
         <v>6</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E48">
+        <v>26</v>
+      </c>
+      <c r="F48" s="1">
+        <v>23.076923076923077</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>2019</v>
       </c>
@@ -1073,8 +1369,14 @@
         <v>6.7</v>
       </c>
       <c r="D49" s="8"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E49">
+        <v>26</v>
+      </c>
+      <c r="F49" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>2019</v>
       </c>
@@ -1087,8 +1389,14 @@
       <c r="D50" s="6">
         <v>7</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E50">
+        <v>26</v>
+      </c>
+      <c r="F50" s="1">
+        <v>26.923076923076923</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>2019</v>
       </c>
@@ -1101,8 +1409,14 @@
       <c r="D51" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E51">
+        <v>26</v>
+      </c>
+      <c r="F51" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>2019</v>
       </c>
@@ -1115,8 +1429,14 @@
       <c r="D52" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E52">
+        <v>26</v>
+      </c>
+      <c r="F52" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>2019</v>
       </c>
@@ -1127,6 +1447,12 @@
         <v>5.8</v>
       </c>
       <c r="D53" s="6">
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <v>26</v>
+      </c>
+      <c r="F53" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>